<commit_message>
R 0.1.7 (Cache, Search)
</commit_message>
<xml_diff>
--- a/data/optimize-genai-2024-0418.xlsx
+++ b/data/optimize-genai-2024-0418.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/manavsehgal/Developer/gtsystem/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06351E48-AE35-DA42-91D8-31D043A1CB0C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E08FAD09-649D-534B-A922-02B68DB4E0C2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1100" yWindow="820" windowWidth="28040" windowHeight="17440" xr2:uid="{B3A12AD0-0ED7-3D48-B84E-F822738D01BF}"/>
   </bookViews>
@@ -56,9 +56,6 @@
     <t>How to scale LLMs efficiently?</t>
   </si>
   <si>
-    <t>What to most effectively deploy LLMs?</t>
-  </si>
-  <si>
     <t>What to perform training data selection and curation for LLMs?</t>
   </si>
   <si>
@@ -123,6 +120,9 @@
   </si>
   <si>
     <t>Only respond with a markdown table with the top 5 latest emerging trends or technologies ranked by order of most popular first. Include columns for Popularity, Emerging Trend or Technology, Description, Recommended by Experts (with 3 top industry analysts or Big5 consultants or VCs recommending the trend or technology), Paper (with link to latest paper about the strategy). Be factual in your response. When facts are not available, do not generate response. Don't explain your response.</t>
+  </si>
+  <si>
+    <t>How to most effectively deploy LLMs?</t>
   </si>
 </sst>
 </file>
@@ -510,7 +510,7 @@
   <dimension ref="A1:C13"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="156" zoomScaleNormal="156" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -523,10 +523,10 @@
   <sheetData>
     <row r="1" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>13</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>14</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>1</v>
@@ -534,10 +534,10 @@
     </row>
     <row r="2" spans="1:3" ht="85" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>2</v>
@@ -545,10 +545,10 @@
     </row>
     <row r="3" spans="1:3" ht="85" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>3</v>
@@ -556,10 +556,10 @@
     </row>
     <row r="4" spans="1:3" ht="85" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>4</v>
@@ -567,21 +567,21 @@
     </row>
     <row r="5" spans="1:3" ht="85" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>6</v>
+        <v>28</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="85" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C6" s="2" t="s">
         <v>5</v>
@@ -589,65 +589,65 @@
     </row>
     <row r="7" spans="1:3" ht="85" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="85" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="85" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="10" spans="1:3" ht="85" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="11" spans="1:3" ht="85" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="12" spans="1:3" ht="85" x14ac:dyDescent="0.2">
       <c r="A12" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C12" s="2" t="s">
         <v>0</v>
@@ -655,13 +655,13 @@
     </row>
     <row r="13" spans="1:3" ht="119" x14ac:dyDescent="0.2">
       <c r="A13" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
   </sheetData>

</xml_diff>